<commit_message>
Descripciones de caso de uso, Excel requerimientos, diagrama de caso de uso
</commit_message>
<xml_diff>
--- a/SAP - TECNOLOGIA/Iteración II/01 - Análisis de Requerimientos/02 - Requerimientos/Requerimientos Funcionales 1.0.xlsx
+++ b/SAP - TECNOLOGIA/Iteración II/01 - Análisis de Requerimientos/02 - Requerimientos/Requerimientos Funcionales 1.0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\SAP-TFI 2015\sap-tfi-documentation\SAP - TECNOLOGIA\Iteración II\01 - Análisis de Requerimientos\02 - Requerimientos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo\Desktop\SAPgit\sap-tfi-documentation\SAP - TECNOLOGIA\Iteración II\01 - Análisis de Requerimientos\02 - Requerimientos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,25 +22,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Código</t>
   </si>
   <si>
     <t>Descripción</t>
+  </si>
+  <si>
+    <t>RF06</t>
+  </si>
+  <si>
+    <t>Se requiere que el usuario confirme el cierre del pedido</t>
+  </si>
+  <si>
+    <t>RF07</t>
+  </si>
+  <si>
+    <t>RF08</t>
+  </si>
+  <si>
+    <t>RF09</t>
+  </si>
+  <si>
+    <t>El usuario tiene que estar logueado para efectivizar el pedido</t>
+  </si>
+  <si>
+    <t>Se requiere notificación al usuario del pedido realizado</t>
+  </si>
+  <si>
+    <t>Se requiere que el usuario pueda modificar la dirección en la cuál se enviará el pedido</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -84,12 +113,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -400,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,28 +453,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4"/>
+    <row r="2" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4"/>
+    <row r="3" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
+    <row r="4" spans="1:2" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
+    <row r="5" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>